<commit_message>
resolve timestamps when import file
</commit_message>
<xml_diff>
--- a/public/GuestsList/data_tamu_smti (1).xlsx
+++ b/public/GuestsList/data_tamu_smti (1).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>No.</t>
   </si>
@@ -32,52 +32,31 @@
     <t>Tujuan</t>
   </si>
   <si>
+    <t>Menemui</t>
+  </si>
+  <si>
     <t>Nomor Telepon</t>
   </si>
   <si>
     <t>Waktu</t>
   </si>
   <si>
-    <t>FIKRI HAYKAL</t>
-  </si>
-  <si>
-    <t>KEMENTRIAN PERINDUSTRIAN</t>
-  </si>
-  <si>
-    <t>Bertemu Pak SUWITO</t>
-  </si>
-  <si>
-    <t>Wednesday, 04-12-2024 16:46:33</t>
-  </si>
-  <si>
-    <t>Tuesday, 03-12-2024 09:29:29</t>
-  </si>
-  <si>
-    <t>Monday, 02-12-2024 16:48:59</t>
-  </si>
-  <si>
-    <t>FIKRI HAYKAL FAHREZA</t>
-  </si>
-  <si>
-    <t>SMK SMTI PONTIANAK</t>
-  </si>
-  <si>
-    <t>BERTEMU KEPSEK</t>
-  </si>
-  <si>
-    <t>08991156396</t>
-  </si>
-  <si>
-    <t>Monday, 02-12-2024 11:21:36</t>
-  </si>
-  <si>
-    <t>Monday, 02-12-2024 11:21:32</t>
-  </si>
-  <si>
-    <t>Koordinasi dengan Guru TOI</t>
-  </si>
-  <si>
-    <t>Monday, 02-12-2024 00:44:05</t>
+    <t>sdwdwd</t>
+  </si>
+  <si>
+    <t>wdwdw</t>
+  </si>
+  <si>
+    <t>dwdwd</t>
+  </si>
+  <si>
+    <t>wdwdwdw</t>
+  </si>
+  <si>
+    <t>Friday, 06-12-2024 15:20:34</t>
+  </si>
+  <si>
+    <t>Friday, 06-12-2024 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -451,10 +430,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:G1"/>
+      <selection activeCell="A1" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -466,9 +445,10 @@
     <col min="5" max="5" width="20" customWidth="true" style="0"/>
     <col min="6" max="6" width="30" customWidth="true" style="0"/>
     <col min="7" max="7" width="30" customWidth="true" style="0"/>
+    <col min="8" max="8" width="30" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -490,143 +470,788 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1234564567892</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1234564567892</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1234564567892</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="B15" s="1">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="B20" s="1">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1">
         <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>24</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>25</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>26</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>28</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>29</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>30</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="1">
+        <v>4242424242</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>